<commit_message>
Added csv files for Yoneda and Henson data
</commit_message>
<xml_diff>
--- a/EDD_Yoneda_data/Yoneda_set2_Metabolomics_data.xlsx
+++ b/EDD_Yoneda_data/Yoneda_set2_Metabolomics_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10314"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vamshij/Desktop/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettroell/Documents/VS_code_projects/OpacusBiodesign/EDD_Yoneda_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB0E93F-A9C8-9C41-866E-7AFB7FAEA5B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB24F3E-6709-0641-8E6B-7B10836179E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14360" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NEW_PROTO" sheetId="4" r:id="rId1"/>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B735FA-75EC-4F45-B634-EDA2C0E7E521}">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>